<commit_message>
Error Calculations and Plots
</commit_message>
<xml_diff>
--- a/data_impute_project/removed_data/human/combination_3_ABCDF/A/10/seed1/missing_data.xlsx
+++ b/data_impute_project/removed_data/human/combination_3_ABCDF/A/10/seed1/missing_data.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F35"/>
+  <dimension ref="A1:F33"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -990,216 +990,170 @@
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>RM 232</t>
+          <t>SC 5</t>
         </is>
       </c>
       <c r="B26" t="n">
-        <v>-19.7</v>
+        <v>-20.2</v>
       </c>
       <c r="C26" t="n">
-        <v>10.7</v>
+        <v>10.8</v>
       </c>
       <c r="D26" t="n">
-        <v>-15.6</v>
+        <v>-13.8</v>
       </c>
       <c r="E26" t="n">
-        <v>-8.800000000000001</v>
-      </c>
-      <c r="F26" t="inlineStr">
-        <is>
-          <t> </t>
-        </is>
+        <v>-5</v>
+      </c>
+      <c r="F26" t="n">
+        <v>17.38</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>SC 5</t>
+          <t>SC 101</t>
         </is>
       </c>
       <c r="B27" t="n">
-        <v>-20.2</v>
+        <v>-20.4</v>
       </c>
       <c r="C27" t="n">
-        <v>10.8</v>
+        <v>10</v>
       </c>
       <c r="D27" t="n">
-        <v>-13.8</v>
+        <v>-14.6</v>
       </c>
       <c r="E27" t="n">
-        <v>-5</v>
+        <v>-10</v>
       </c>
       <c r="F27" t="n">
-        <v>17.38</v>
+        <v>17</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>SC 92</t>
+          <t>SC 105</t>
         </is>
       </c>
       <c r="B28" t="inlineStr"/>
       <c r="C28" t="n">
-        <v>14.3</v>
+        <v>11.1</v>
       </c>
       <c r="D28" t="n">
-        <v>-14</v>
+        <v>-13.7</v>
       </c>
       <c r="E28" t="n">
-        <v>-6.3</v>
+        <v>-5.9</v>
       </c>
       <c r="F28" t="n">
-        <v>17.22</v>
+        <v>17.44</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>SC 101</t>
+          <t>SC 119</t>
         </is>
       </c>
       <c r="B29" t="inlineStr"/>
       <c r="C29" t="n">
-        <v>10</v>
+        <v>11.2</v>
       </c>
       <c r="D29" t="n">
-        <v>-14.6</v>
+        <v>-13</v>
       </c>
       <c r="E29" t="n">
-        <v>-10</v>
+        <v>-6.8</v>
       </c>
       <c r="F29" t="n">
-        <v>17</v>
+        <v>18.06</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>SC 105</t>
+          <t>SC 120</t>
         </is>
       </c>
       <c r="B30" t="n">
-        <v>-19.6</v>
+        <v>-19.7</v>
       </c>
       <c r="C30" t="n">
-        <v>11.1</v>
+        <v>11.4</v>
       </c>
       <c r="D30" t="n">
-        <v>-13.7</v>
+        <v>-13.6</v>
       </c>
       <c r="E30" t="n">
-        <v>-5.9</v>
+        <v>-5.7</v>
       </c>
       <c r="F30" t="n">
-        <v>17.44</v>
+        <v>16.89</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>SC 119</t>
+          <t>SC 132</t>
         </is>
       </c>
       <c r="B31" t="n">
-        <v>-19.5</v>
+        <v>-18.8</v>
       </c>
       <c r="C31" t="n">
-        <v>11.2</v>
+        <v>15.3</v>
       </c>
       <c r="D31" t="n">
-        <v>-13</v>
+        <v>-13.7</v>
       </c>
       <c r="E31" t="n">
-        <v>-6.8</v>
+        <v>-8.1</v>
       </c>
       <c r="F31" t="n">
-        <v>18.06</v>
+        <v>17.18</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>SC 120</t>
+          <t>SC 193</t>
         </is>
       </c>
       <c r="B32" t="inlineStr"/>
       <c r="C32" t="n">
-        <v>11.4</v>
+        <v>10.5</v>
       </c>
       <c r="D32" t="n">
-        <v>-13.6</v>
+        <v>-14.7</v>
       </c>
       <c r="E32" t="n">
-        <v>-5.7</v>
+        <v>-6.4</v>
       </c>
       <c r="F32" t="n">
-        <v>16.89</v>
+        <v>17.39</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>SC 132</t>
+          <t>SC 232</t>
         </is>
       </c>
       <c r="B33" t="n">
-        <v>-18.8</v>
+        <v>-19.5</v>
       </c>
       <c r="C33" t="n">
-        <v>15.3</v>
+        <v>10.4</v>
       </c>
       <c r="D33" t="n">
-        <v>-13.7</v>
+        <v>-14.1</v>
       </c>
       <c r="E33" t="n">
-        <v>-8.1</v>
+        <v>-10.7</v>
       </c>
       <c r="F33" t="n">
-        <v>17.18</v>
-      </c>
-    </row>
-    <row r="34">
-      <c r="A34" t="inlineStr">
-        <is>
-          <t>SC 193</t>
-        </is>
-      </c>
-      <c r="B34" t="n">
-        <v>-19.9</v>
-      </c>
-      <c r="C34" t="n">
-        <v>10.5</v>
-      </c>
-      <c r="D34" t="n">
-        <v>-14.7</v>
-      </c>
-      <c r="E34" t="n">
-        <v>-6.4</v>
-      </c>
-      <c r="F34" t="n">
-        <v>17.39</v>
-      </c>
-    </row>
-    <row r="35">
-      <c r="A35" t="inlineStr">
-        <is>
-          <t>SC 232</t>
-        </is>
-      </c>
-      <c r="B35" t="n">
-        <v>-19.5</v>
-      </c>
-      <c r="C35" t="n">
-        <v>10.4</v>
-      </c>
-      <c r="D35" t="n">
-        <v>-14.1</v>
-      </c>
-      <c r="E35" t="n">
-        <v>-10.7</v>
-      </c>
-      <c r="F35" t="n">
         <v>17.53</v>
       </c>
     </row>

</xml_diff>